<commit_message>
Translation (EST) + doi
</commit_message>
<xml_diff>
--- a/translations/translation_est.xlsx
+++ b/translations/translation_est.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcadmin\Documents\dok\TARU\PROJEKTID\EEGManyLabs\Task\spotlight_replication\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057B97CB-6CAE-40E3-BF9D-F472F85977D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDCB3A6-BB74-4C10-A695-4A454A53E11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,10 +85,6 @@
 Katsega alustamiseks vajutage palu "tühikut"…</t>
   </si>
   <si>
-    <t>Tere tulemast ja aitäh, et nõustusite osalema meie eksperimendis!\n\n
-See uuring on osa rahvusvahelisest algatusest #EEGManyLabs, mille eesmärk on uurida ligikaudu 20 mõjuka kognitiiv-neuroteadusliku EEG-uuringu korratavust. Selles eksperimendis kordame ja laiendame Professor Matthias M. Mülleri ja tema kolleegide 2003. aastal läbi viidud ruumilise tähelepanu uuringut.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Keskenduge palun asukohtadele: </t>
   </si>
   <si>
@@ -109,6 +105,10 @@
 (1) Millistele ruutudele tähelepanu pöörata.\n
 (2) Millist kätt vastamiseks kasutada.\n
 Iga ploki poole peal palutakse teil käsi vahetada.</t>
+  </si>
+  <si>
+    <t>Tere tulemast ja aitäh, et nõustusite osalema meie eksperimendis!\n\n
+See uuring on osa rahvusvahelisest algatusest #EEGManyLabs, mille eesmärk on uurida ligikaudu 20 mõjuka kognitiiv-neuroteadusliku EEG-uuringu korratavust. Selles eksperimendis kordame ja laiendame professor Matthias M. Mülleri ja tema kolleegide 2003. aastal läbi viidud ruumilise tähelepanu uuringut.</t>
   </si>
 </sst>
 </file>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -510,7 +510,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -518,7 +518,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>